<commit_message>
Added generation of mecDict and serviceDict in Scenario.py
</commit_message>
<xml_diff>
--- a/Code/file/input/scenario_1.xlsx
+++ b/Code/file/input/scenario_1.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="mec" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="service" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="request" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="intervalForSendingRequests" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t xml:space="preserve">computer power</t>
   </si>
@@ -49,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">s3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interval for sending requests</t>
   </si>
 </sst>
 </file>
@@ -152,7 +156,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.48"/>
   </cols>
@@ -208,7 +212,7 @@
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
@@ -269,11 +273,11 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
@@ -326,6 +330,41 @@
       </c>
       <c r="D4" s="0" t="n">
         <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;KffffffPágina &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.28"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="0" t="n">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified the preferential queue. The request is shifted to the left to get additional free space on the right.
</commit_message>
<xml_diff>
--- a/Code/file/input/scenario_1.xlsx
+++ b/Code/file/input/scenario_1.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t xml:space="preserve">computerPower</t>
   </si>
@@ -50,6 +50,15 @@
   </si>
   <si>
     <t xml:space="preserve">s3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s6</t>
   </si>
   <si>
     <t xml:space="preserve">intervalForSendingRequests</t>
@@ -128,8 +137,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -153,10 +166,10 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.48"/>
   </cols>
@@ -171,7 +184,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>1111</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -179,7 +192,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>2222</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -187,7 +200,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>3333</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -206,13 +219,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.51"/>
   </cols>
@@ -225,37 +238,70 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>111</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>90</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>222</v>
-      </c>
-      <c r="C3" s="0" t="n">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="1" t="n">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>333</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>33</v>
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>
@@ -274,15 +320,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
         <v>6</v>
       </c>
@@ -291,6 +337,15 @@
       </c>
       <c r="D1" s="0" t="s">
         <v>8</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -298,41 +353,68 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>11</v>
+        <v>700</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>12</v>
+        <v>500</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>200</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>21</v>
+        <v>200</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>22</v>
+        <v>400</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>700</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>31</v>
+        <v>400</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>32</v>
+        <v>700</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>33</v>
+        <v>200</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>400</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -354,20 +436,20 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.28"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>200</v>
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>120000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created main2 for summary statistics
</commit_message>
<xml_diff>
--- a/Code/file/input/scenario_1.xlsx
+++ b/Code/file/input/scenario_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="mec" sheetId="1" state="visible" r:id="rId2"/>
@@ -169,7 +169,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.48"/>
   </cols>
@@ -222,10 +222,10 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.51"/>
   </cols>
@@ -243,10 +243,10 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>3000</v>
+        <v>9000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -254,10 +254,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>3000</v>
+        <v>9000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -265,10 +265,10 @@
         <v>8</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>3000</v>
+        <v>9000</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -276,10 +276,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>2000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -287,10 +287,10 @@
         <v>10</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>2000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -298,10 +298,10 @@
         <v>11</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>2000</v>
+        <v>4000</v>
       </c>
     </row>
   </sheetData>
@@ -322,11 +322,11 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
@@ -353,19 +353,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>200</v>
@@ -379,19 +379,19 @@
         <v>200</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>200</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>700</v>
+        <v>500</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -399,19 +399,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>200</v>
@@ -435,11 +435,11 @@
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.28"/>
   </cols>

</xml_diff>